<commit_message>
SoGo NS reading issues and DMX DP issues are fixed
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_NSReadings.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_NSReadings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0ADD38-E89C-4CFD-8440-8D58CD8B1339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A00F089-E03E-404F-8DC8-EAD59AAE5FF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="75">
   <si>
     <t>Environment</t>
   </si>
@@ -247,10 +247,7 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>7.76</t>
-  </si>
-  <si>
-    <t>8.81</t>
+    <t>13.84</t>
   </si>
 </sst>
 </file>
@@ -258,7 +255,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,8 +327,184 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="114">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +525,486 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -461,7 +1114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -480,6 +1133,70 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="43" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="45" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="47" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="49" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="51" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="53" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="55" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="57" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="59" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="61" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="63" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="65" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="67" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="69" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="28" fillId="71" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="73" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="75" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="77" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="79" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="81" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="32" fillId="83" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="85" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="87" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="89" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="91" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="93" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="36" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="97" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="99" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="38" fillId="101" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="103" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="40" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="109" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="111" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="113" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -918,7 +1635,7 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +1710,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -1014,11 +1731,11 @@
       <c r="I2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>73</v>
+      <c r="J2" s="72" t="s">
+        <v>70</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="4"/>
@@ -1054,7 +1771,7 @@
       <c r="I3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -1096,7 +1813,7 @@
       <c r="I4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K4" s="5" t="s">
@@ -1138,7 +1855,7 @@
       <c r="I5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -1180,7 +1897,7 @@
       <c r="I6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -1222,7 +1939,7 @@
       <c r="I7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -1264,7 +1981,7 @@
       <c r="I8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="80" t="s">
         <v>70</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -1306,7 +2023,7 @@
       <c r="I9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -1348,7 +2065,7 @@
       <c r="I10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -1390,7 +2107,7 @@
       <c r="I11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1432,7 +2149,7 @@
       <c r="I12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="72" t="s">
         <v>70</v>
       </c>
       <c r="K12" s="5" t="s">

</xml_diff>